<commit_message>
Rename di Person in Contact [piallare DB]
</commit_message>
<xml_diff>
--- a/Questionari Excel/Questionario Data Entry.xlsx
+++ b/Questionari Excel/Questionario Data Entry.xlsx
@@ -838,16 +838,16 @@
         <v>9</v>
       </c>
       <c r="T2" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="U2" s="3">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="V2" s="3">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="W2" s="3">
-        <v>258</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -870,10 +870,10 @@
         <v>9</v>
       </c>
       <c r="V3" s="3">
-        <v>127</v>
+        <v>2</v>
       </c>
       <c r="W3" s="3">
-        <v>259</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -896,10 +896,10 @@
         <v>9</v>
       </c>
       <c r="V4" s="3">
-        <v>128</v>
+        <v>3</v>
       </c>
       <c r="W4" s="3">
-        <v>260</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -934,16 +934,16 @@
         <v>3</v>
       </c>
       <c r="T5" s="3">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="U5" s="3">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="V5" s="3">
-        <v>129</v>
+        <v>4</v>
       </c>
       <c r="W5" s="3">
-        <v>261</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -963,7 +963,7 @@
         <v>3</v>
       </c>
       <c r="W6" s="3">
-        <v>262</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -983,7 +983,7 @@
         <v>5</v>
       </c>
       <c r="W7" s="3">
-        <v>263</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -1003,7 +1003,7 @@
         <v>5</v>
       </c>
       <c r="W8" s="3">
-        <v>264</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -1023,7 +1023,7 @@
         <v>5</v>
       </c>
       <c r="W9" s="3">
-        <v>265</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -1043,7 +1043,7 @@
         <v>5</v>
       </c>
       <c r="W10" s="3">
-        <v>266</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -1063,7 +1063,7 @@
         <v>2</v>
       </c>
       <c r="W11" s="3">
-        <v>267</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -1083,7 +1083,7 @@
         <v>2</v>
       </c>
       <c r="W12" s="3">
-        <v>268</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -1106,10 +1106,10 @@
         <v>2</v>
       </c>
       <c r="V13" s="3">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="W13" s="3">
-        <v>269</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -1138,13 +1138,13 @@
         <v>1</v>
       </c>
       <c r="U14" s="3">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="V14" s="3">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="W14" s="3">
-        <v>270</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -1161,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="W15" s="3">
-        <v>271</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -1178,7 +1178,7 @@
         <v>8</v>
       </c>
       <c r="W16" s="3">
-        <v>272</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
@@ -1207,13 +1207,13 @@
         <v>1</v>
       </c>
       <c r="U17" s="3">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="V17" s="3">
-        <v>132</v>
+        <v>7</v>
       </c>
       <c r="W17" s="3">
-        <v>273</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -1230,7 +1230,7 @@
         <v>9</v>
       </c>
       <c r="W18" s="3">
-        <v>274</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -1262,13 +1262,13 @@
         <v>5</v>
       </c>
       <c r="U19" s="3">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="V19" s="3">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="W19" s="3">
-        <v>275</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
@@ -1291,10 +1291,10 @@
         <v>9</v>
       </c>
       <c r="V20" s="3">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="W20" s="3">
-        <v>276</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
@@ -1317,10 +1317,10 @@
         <v>9</v>
       </c>
       <c r="V21" s="3">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="W21" s="3">
-        <v>277</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -1343,10 +1343,10 @@
         <v>7</v>
       </c>
       <c r="V22" s="3">
-        <v>136</v>
+        <v>11</v>
       </c>
       <c r="W22" s="3">
-        <v>278</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23">
@@ -1369,10 +1369,10 @@
         <v>9</v>
       </c>
       <c r="V23" s="3">
-        <v>137</v>
+        <v>12</v>
       </c>
       <c r="W23" s="3">
-        <v>279</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -1395,10 +1395,10 @@
         <v>9</v>
       </c>
       <c r="V24" s="3">
-        <v>138</v>
+        <v>13</v>
       </c>
       <c r="W24" s="3">
-        <v>280</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25">
@@ -1421,10 +1421,10 @@
         <v>1</v>
       </c>
       <c r="V25" s="3">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="W25" s="3">
-        <v>281</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
@@ -1456,13 +1456,13 @@
         <v>9</v>
       </c>
       <c r="U26" s="3">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="V26" s="3">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="W26" s="3">
-        <v>282</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27">
@@ -1485,10 +1485,10 @@
         <v>9</v>
       </c>
       <c r="V27" s="3">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="W27" s="3">
-        <v>283</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28">
@@ -1511,10 +1511,10 @@
         <v>9</v>
       </c>
       <c r="V28" s="3">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="W28" s="3">
-        <v>284</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29">
@@ -1543,13 +1543,13 @@
         <v>1</v>
       </c>
       <c r="U29" s="3">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="V29" s="3">
-        <v>143</v>
+        <v>18</v>
       </c>
       <c r="W29" s="3">
-        <v>285</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30">
@@ -1566,7 +1566,7 @@
         <v>3</v>
       </c>
       <c r="W30" s="3">
-        <v>286</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31">
@@ -1583,7 +1583,7 @@
         <v>6</v>
       </c>
       <c r="W31" s="3">
-        <v>287</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32">
@@ -1600,7 +1600,7 @@
         <v>8</v>
       </c>
       <c r="W32" s="3">
-        <v>288</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33">
@@ -1635,16 +1635,16 @@
         <v>9</v>
       </c>
       <c r="T33" s="3">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="U33" s="3">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="V33" s="3">
-        <v>144</v>
+        <v>19</v>
       </c>
       <c r="W33" s="3">
-        <v>289</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34">
@@ -1667,10 +1667,10 @@
         <v>1</v>
       </c>
       <c r="V34" s="3">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="W34" s="3">
-        <v>290</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35">
@@ -1693,10 +1693,10 @@
         <v>9</v>
       </c>
       <c r="V35" s="3">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="W35" s="3">
-        <v>291</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36">
@@ -1731,13 +1731,13 @@
         <v>2</v>
       </c>
       <c r="U36" s="3">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="V36" s="3">
-        <v>147</v>
+        <v>22</v>
       </c>
       <c r="W36" s="3">
-        <v>292</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37">
@@ -1757,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="W37" s="3">
-        <v>293</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38">
@@ -1777,7 +1777,7 @@
         <v>7</v>
       </c>
       <c r="W38" s="3">
-        <v>294</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39">
@@ -1797,7 +1797,7 @@
         <v>7</v>
       </c>
       <c r="W39" s="3">
-        <v>295</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40">
@@ -1817,7 +1817,7 @@
         <v>9</v>
       </c>
       <c r="W40" s="3">
-        <v>296</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41">
@@ -1837,7 +1837,7 @@
         <v>9</v>
       </c>
       <c r="W41" s="3">
-        <v>297</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42">
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="W42" s="3">
-        <v>298</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43">
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="W43" s="3">
-        <v>299</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44">
@@ -1900,10 +1900,10 @@
         <v>9</v>
       </c>
       <c r="V44" s="3">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="W44" s="3">
-        <v>300</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45">
@@ -1929,10 +1929,10 @@
         <v>2</v>
       </c>
       <c r="V45" s="3">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="W45" s="3">
-        <v>301</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46">
@@ -1952,7 +1952,7 @@
         <v>2</v>
       </c>
       <c r="W46" s="3">
-        <v>302</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47">
@@ -1972,7 +1972,7 @@
         <v>7</v>
       </c>
       <c r="W47" s="3">
-        <v>303</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48">
@@ -1992,7 +1992,7 @@
         <v>7</v>
       </c>
       <c r="W48" s="3">
-        <v>304</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49">
@@ -2012,7 +2012,7 @@
         <v>9</v>
       </c>
       <c r="W49" s="3">
-        <v>305</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50">
@@ -2032,7 +2032,7 @@
         <v>9</v>
       </c>
       <c r="W50" s="3">
-        <v>306</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51">
@@ -2052,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="W51" s="3">
-        <v>307</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52">
@@ -2072,7 +2072,7 @@
         <v>1</v>
       </c>
       <c r="W52" s="3">
-        <v>308</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53">
@@ -2098,10 +2098,10 @@
         <v>3</v>
       </c>
       <c r="V53" s="3">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="W53" s="3">
-        <v>309</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54">
@@ -2121,7 +2121,7 @@
         <v>3</v>
       </c>
       <c r="W54" s="3">
-        <v>310</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55">
@@ -2141,7 +2141,7 @@
         <v>8</v>
       </c>
       <c r="W55" s="3">
-        <v>311</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56">
@@ -2161,7 +2161,7 @@
         <v>8</v>
       </c>
       <c r="W56" s="3">
-        <v>312</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57">
@@ -2181,7 +2181,7 @@
         <v>9</v>
       </c>
       <c r="W57" s="3">
-        <v>313</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58">
@@ -2201,7 +2201,7 @@
         <v>9</v>
       </c>
       <c r="W58" s="3">
-        <v>314</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59">
@@ -2221,7 +2221,7 @@
         <v>2</v>
       </c>
       <c r="W59" s="3">
-        <v>315</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60">
@@ -2241,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="W60" s="3">
-        <v>316</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61">
@@ -2276,16 +2276,16 @@
         <v>9</v>
       </c>
       <c r="T61" s="3">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="U61" s="3">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="V61" s="3">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="W61" s="3">
-        <v>317</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62">
@@ -2308,10 +2308,10 @@
         <v>9</v>
       </c>
       <c r="V62" s="3">
-        <v>152</v>
+        <v>27</v>
       </c>
       <c r="W62" s="3">
-        <v>318</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63">
@@ -2334,10 +2334,10 @@
         <v>1</v>
       </c>
       <c r="V63" s="3">
-        <v>153</v>
+        <v>28</v>
       </c>
       <c r="W63" s="3">
-        <v>319</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64">
@@ -2360,10 +2360,10 @@
         <v>9</v>
       </c>
       <c r="V64" s="3">
-        <v>154</v>
+        <v>29</v>
       </c>
       <c r="W64" s="3">
-        <v>320</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65">
@@ -2395,13 +2395,13 @@
         <v>7</v>
       </c>
       <c r="U65" s="3">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="V65" s="3">
-        <v>155</v>
+        <v>30</v>
       </c>
       <c r="W65" s="3">
-        <v>321</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66">
@@ -2424,10 +2424,10 @@
         <v>1</v>
       </c>
       <c r="V66" s="3">
-        <v>156</v>
+        <v>31</v>
       </c>
       <c r="W66" s="3">
-        <v>322</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67">
@@ -2450,10 +2450,10 @@
         <v>7</v>
       </c>
       <c r="V67" s="3">
-        <v>157</v>
+        <v>32</v>
       </c>
       <c r="W67" s="3">
-        <v>323</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68">
@@ -2482,13 +2482,13 @@
         <v>1</v>
       </c>
       <c r="U68" s="3">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="V68" s="3">
-        <v>158</v>
+        <v>33</v>
       </c>
       <c r="W68" s="3">
-        <v>324</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69">
@@ -2505,7 +2505,7 @@
         <v>5</v>
       </c>
       <c r="W69" s="3">
-        <v>325</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70">
@@ -2534,13 +2534,13 @@
         <v>5</v>
       </c>
       <c r="U70" s="3">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="V70" s="3">
-        <v>159</v>
+        <v>34</v>
       </c>
       <c r="W70" s="3">
-        <v>326</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71">
@@ -2557,7 +2557,7 @@
         <v>8</v>
       </c>
       <c r="W71" s="3">
-        <v>327</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72">
@@ -2586,13 +2586,13 @@
         <v>1</v>
       </c>
       <c r="U72" s="3">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="V72" s="3">
-        <v>160</v>
+        <v>35</v>
       </c>
       <c r="W72" s="3">
-        <v>328</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73">
@@ -2609,7 +2609,7 @@
         <v>7</v>
       </c>
       <c r="W73" s="3">
-        <v>329</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74">
@@ -2641,16 +2641,16 @@
         <v>1</v>
       </c>
       <c r="T74" s="3">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="U74" s="3">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="V74" s="3">
-        <v>161</v>
+        <v>36</v>
       </c>
       <c r="W74" s="3">
-        <v>330</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75">
@@ -2667,7 +2667,7 @@
         <v>9</v>
       </c>
       <c r="W75" s="3">
-        <v>331</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76">
@@ -2696,13 +2696,13 @@
         <v>1</v>
       </c>
       <c r="U76" s="3">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="V76" s="3">
-        <v>162</v>
+        <v>37</v>
       </c>
       <c r="W76" s="3">
-        <v>332</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77">
@@ -2719,7 +2719,7 @@
         <v>9</v>
       </c>
       <c r="W77" s="3">
-        <v>333</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78">
@@ -2748,13 +2748,13 @@
         <v>1</v>
       </c>
       <c r="U78" s="3">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="V78" s="3">
-        <v>163</v>
+        <v>38</v>
       </c>
       <c r="W78" s="3">
-        <v>334</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79">
@@ -2771,7 +2771,7 @@
         <v>9</v>
       </c>
       <c r="W79" s="3">
-        <v>335</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80">
@@ -2800,13 +2800,13 @@
         <v>1</v>
       </c>
       <c r="U80" s="3">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="V80" s="3">
-        <v>164</v>
+        <v>39</v>
       </c>
       <c r="W80" s="3">
-        <v>336</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81">
@@ -2823,7 +2823,7 @@
         <v>9</v>
       </c>
       <c r="W81" s="3">
-        <v>337</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82">
@@ -2852,13 +2852,13 @@
         <v>9</v>
       </c>
       <c r="U82" s="3">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="V82" s="3">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="W82" s="3">
-        <v>338</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83">
@@ -2875,7 +2875,7 @@
         <v>1</v>
       </c>
       <c r="W83" s="3">
-        <v>339</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84">
@@ -2904,13 +2904,13 @@
         <v>1</v>
       </c>
       <c r="U84" s="3">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="V84" s="3">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="W84" s="3">
-        <v>340</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85">
@@ -2927,7 +2927,7 @@
         <v>9</v>
       </c>
       <c r="W85" s="3">
-        <v>341</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86">
@@ -2956,13 +2956,13 @@
         <v>9</v>
       </c>
       <c r="U86" s="3">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="V86" s="3">
-        <v>167</v>
+        <v>42</v>
       </c>
       <c r="W86" s="3">
-        <v>342</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87">
@@ -2979,7 +2979,7 @@
         <v>9</v>
       </c>
       <c r="W87" s="3">
-        <v>343</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88">
@@ -2996,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="W88" s="3">
-        <v>344</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89">
@@ -3013,7 +3013,7 @@
         <v>1</v>
       </c>
       <c r="W89" s="3">
-        <v>345</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90">
@@ -3042,13 +3042,13 @@
         <v>1</v>
       </c>
       <c r="U90" s="3">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="V90" s="3">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="W90" s="3">
-        <v>346</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91">
@@ -3065,7 +3065,7 @@
         <v>9</v>
       </c>
       <c r="W91" s="3">
-        <v>347</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92">
@@ -3094,13 +3094,13 @@
         <v>1</v>
       </c>
       <c r="U92" s="3">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="V92" s="3">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="W92" s="3">
-        <v>348</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93">
@@ -3117,7 +3117,7 @@
         <v>9</v>
       </c>
       <c r="W93" s="3">
-        <v>349</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix richieste per questionario
</commit_message>
<xml_diff>
--- a/Questionari Excel/Questionario Data Entry.xlsx
+++ b/Questionari Excel/Questionario Data Entry.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larks\Documents\GitHub\MyGenomics\Questionari Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larks\Documents\MyGenomics\Questionari Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Categoria Domanda</t>
   </si>
@@ -64,7 +64,7 @@
     <t>ANALISI ALIMENTARE</t>
   </si>
   <si>
-    <t>Ha alcune dei seguenti fastidi?</t>
+    <t>Ha alcune dei seguenti problemi?</t>
   </si>
   <si>
     <t>SI</t>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>VEROFALSO</t>
+  </si>
+  <si>
+    <t>TUTTI</t>
   </si>
   <si>
     <t>NUTRIGENOMICA</t>
@@ -367,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +407,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -417,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
@@ -428,6 +437,7 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="5" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="6" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="7" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -723,24 +733,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -751,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W93"/>
+  <dimension ref="A1:W97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,8 +836,11 @@
       <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="4">
         <v>0</v>
@@ -853,13 +866,16 @@
     </row>
     <row r="3">
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G3" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" s="4">
         <v>0</v>
@@ -885,13 +901,16 @@
     </row>
     <row r="4">
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I4" s="4">
         <v>0</v>
@@ -915,59 +934,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="5" s="10" customFormat="1">
+      <c r="T5" s="10">
+        <v>1</v>
+      </c>
+      <c r="U5" s="10">
+        <v>1</v>
+      </c>
+      <c r="V5" s="10">
+        <v>3</v>
+      </c>
+      <c r="W5" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>3</v>
-      </c>
-      <c r="T5" s="4">
-        <v>2</v>
-      </c>
-      <c r="U5" s="4">
-        <v>2</v>
-      </c>
-      <c r="V5" s="4">
-        <v>4</v>
-      </c>
-      <c r="W5" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
       <c r="G6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
@@ -978,17 +982,17 @@
       <c r="K6" s="4">
         <v>3</v>
       </c>
-      <c r="T6" s="2">
-        <v>2</v>
-      </c>
-      <c r="U6" s="2">
-        <v>2</v>
-      </c>
-      <c r="V6" s="2">
+      <c r="T6" s="4">
+        <v>2</v>
+      </c>
+      <c r="U6" s="4">
+        <v>2</v>
+      </c>
+      <c r="V6" s="4">
         <v>4</v>
       </c>
       <c r="W6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -996,7 +1000,7 @@
         <v>26</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I7" s="4">
         <v>0</v>
@@ -1005,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T7" s="2">
         <v>2</v>
@@ -1017,7 +1021,7 @@
         <v>4</v>
       </c>
       <c r="W7" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -1025,7 +1029,7 @@
         <v>27</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I8" s="4">
         <v>0</v>
@@ -1046,7 +1050,7 @@
         <v>4</v>
       </c>
       <c r="W8" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -1054,7 +1058,7 @@
         <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I9" s="4">
         <v>0</v>
@@ -1075,7 +1079,7 @@
         <v>4</v>
       </c>
       <c r="W9" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -1083,7 +1087,7 @@
         <v>29</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I10" s="4">
         <v>0</v>
@@ -1104,7 +1108,7 @@
         <v>4</v>
       </c>
       <c r="W10" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -1112,7 +1116,7 @@
         <v>30</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I11" s="4">
         <v>0</v>
@@ -1121,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T11" s="2">
         <v>2</v>
@@ -1133,7 +1137,7 @@
         <v>4</v>
       </c>
       <c r="W11" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -1141,7 +1145,7 @@
         <v>31</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I12" s="4">
         <v>0</v>
@@ -1162,117 +1166,129 @@
         <v>4</v>
       </c>
       <c r="W12" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="G13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2</v>
+      </c>
+      <c r="T13" s="2">
+        <v>2</v>
+      </c>
+      <c r="U13" s="2">
+        <v>2</v>
+      </c>
+      <c r="V13" s="2">
+        <v>4</v>
+      </c>
+      <c r="W13" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="13">
-      <c r="E13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="4" t="s">
+    <row r="14">
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>2</v>
-      </c>
-      <c r="T13" s="2">
-        <v>2</v>
-      </c>
-      <c r="U13" s="2">
-        <v>2</v>
-      </c>
-      <c r="V13" s="4">
+      <c r="G14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2</v>
+      </c>
+      <c r="T14" s="2">
+        <v>2</v>
+      </c>
+      <c r="U14" s="2">
+        <v>2</v>
+      </c>
+      <c r="V14" s="4">
         <v>5</v>
       </c>
-      <c r="W13" s="4">
+      <c r="W14" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="4" t="s">
+    <row r="15">
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
+      <c r="F15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
         <v>1</v>
       </c>
-      <c r="T14" s="2">
-        <v>2</v>
-      </c>
-      <c r="U14" s="4">
-        <v>3</v>
-      </c>
-      <c r="V14" s="4">
+      <c r="T15" s="2">
+        <v>2</v>
+      </c>
+      <c r="U15" s="4">
+        <v>3</v>
+      </c>
+      <c r="V15" s="4">
         <v>6</v>
       </c>
-      <c r="W14" s="4">
+      <c r="W15" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="15">
-      <c r="H15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="4">
+    <row r="16">
+      <c r="G16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="4">
         <v>1</v>
       </c>
-      <c r="J15" s="4">
-        <v>2</v>
-      </c>
-      <c r="K15" s="4">
-        <v>2</v>
-      </c>
-      <c r="T15" s="2">
-        <v>2</v>
-      </c>
-      <c r="U15" s="2">
-        <v>3</v>
-      </c>
-      <c r="V15" s="2">
-        <v>6</v>
-      </c>
-      <c r="W15" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="H16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="4">
-        <v>3</v>
-      </c>
       <c r="J16" s="4">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="K16" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="T16" s="2">
         <v>2</v>
@@ -1284,123 +1300,129 @@
         <v>6</v>
       </c>
       <c r="W16" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="G17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="4">
+        <v>3</v>
+      </c>
+      <c r="J17" s="4">
+        <v>30</v>
+      </c>
+      <c r="K17" s="4">
+        <v>8</v>
+      </c>
+      <c r="T17" s="2">
+        <v>2</v>
+      </c>
+      <c r="U17" s="2">
+        <v>3</v>
+      </c>
+      <c r="V17" s="2">
+        <v>6</v>
+      </c>
+      <c r="W17" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="4" t="s">
+    <row r="18">
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
+      <c r="G18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
         <v>1</v>
       </c>
-      <c r="T17" s="2">
-        <v>2</v>
-      </c>
-      <c r="U17" s="4">
+      <c r="T18" s="2">
+        <v>2</v>
+      </c>
+      <c r="U18" s="4">
         <v>4</v>
       </c>
-      <c r="V17" s="4">
+      <c r="V18" s="4">
         <v>7</v>
       </c>
-      <c r="W17" s="4">
+      <c r="W18" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="18">
-      <c r="H18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="4">
+    <row r="19">
+      <c r="G19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="4">
         <v>1</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J19" s="4">
         <v>100</v>
       </c>
-      <c r="K18" s="4">
-        <v>9</v>
-      </c>
-      <c r="T18" s="2">
-        <v>2</v>
-      </c>
-      <c r="U18" s="2">
+      <c r="K19" s="4">
+        <v>9</v>
+      </c>
+      <c r="T19" s="2">
+        <v>2</v>
+      </c>
+      <c r="U19" s="2">
         <v>4</v>
       </c>
-      <c r="V18" s="2">
+      <c r="V19" s="2">
         <v>7</v>
       </c>
-      <c r="W18" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="W19" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0</v>
-      </c>
-      <c r="K19" s="4">
-        <v>5</v>
-      </c>
-      <c r="T19" s="2">
-        <v>2</v>
-      </c>
-      <c r="U19" s="4">
-        <v>5</v>
-      </c>
-      <c r="V19" s="4">
-        <v>8</v>
-      </c>
-      <c r="W19" s="4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="D20" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="E20" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G20" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H20" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
@@ -1409,19 +1431,19 @@
         <v>0</v>
       </c>
       <c r="K20" s="4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="T20" s="2">
         <v>2</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U20" s="4">
         <v>5</v>
       </c>
       <c r="V20" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W20" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
@@ -1431,8 +1453,11 @@
       <c r="F21" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G21" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H21" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
@@ -1450,10 +1475,10 @@
         <v>5</v>
       </c>
       <c r="V21" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W21" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -1463,8 +1488,11 @@
       <c r="F22" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G22" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H22" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
@@ -1473,7 +1501,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="T22" s="2">
         <v>2</v>
@@ -1482,10 +1510,10 @@
         <v>5</v>
       </c>
       <c r="V22" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W22" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
@@ -1495,8 +1523,11 @@
       <c r="F23" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G23" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H23" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I23" s="4">
         <v>0</v>
@@ -1505,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T23" s="2">
         <v>2</v>
@@ -1514,10 +1545,10 @@
         <v>5</v>
       </c>
       <c r="V23" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W23" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24">
@@ -1527,8 +1558,11 @@
       <c r="F24" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G24" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H24" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
@@ -1546,10 +1580,10 @@
         <v>5</v>
       </c>
       <c r="V24" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W24" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
@@ -1559,8 +1593,11 @@
       <c r="F25" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G25" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H25" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I25" s="4">
         <v>0</v>
@@ -1569,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T25" s="2">
         <v>2</v>
@@ -1578,30 +1615,24 @@
         <v>5</v>
       </c>
       <c r="V25" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W25" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G26" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H26" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
@@ -1610,30 +1641,42 @@
         <v>0</v>
       </c>
       <c r="K26" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="T26" s="2">
         <v>2</v>
       </c>
-      <c r="U26" s="4">
-        <v>6</v>
+      <c r="U26" s="2">
+        <v>5</v>
       </c>
       <c r="V26" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W26" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
+      <c r="B27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="E27" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G27" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H27" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
@@ -1647,14 +1690,14 @@
       <c r="T27" s="2">
         <v>2</v>
       </c>
-      <c r="U27" s="2">
+      <c r="U27" s="4">
         <v>6</v>
       </c>
       <c r="V27" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W27" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
@@ -1664,8 +1707,11 @@
       <c r="F28" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G28" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H28" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I28" s="4">
         <v>0</v>
@@ -1683,88 +1729,103 @@
         <v>6</v>
       </c>
       <c r="V28" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W28" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <v>9</v>
+      </c>
+      <c r="T29" s="2">
+        <v>2</v>
+      </c>
+      <c r="U29" s="2">
+        <v>6</v>
+      </c>
+      <c r="V29" s="4">
+        <v>17</v>
+      </c>
+      <c r="W29" s="4">
         <v>27</v>
       </c>
     </row>
-    <row r="29">
-      <c r="B29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="4" t="s">
+    <row r="30">
+      <c r="B30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="4">
-        <v>0</v>
-      </c>
-      <c r="J29" s="4">
-        <v>0</v>
-      </c>
-      <c r="K29" s="4">
+      <c r="F30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
         <v>1</v>
       </c>
-      <c r="T29" s="2">
-        <v>2</v>
-      </c>
-      <c r="U29" s="4">
+      <c r="T30" s="2">
+        <v>2</v>
+      </c>
+      <c r="U30" s="4">
         <v>7</v>
       </c>
-      <c r="V29" s="4">
-        <v>18</v>
-      </c>
-      <c r="W29" s="4">
+      <c r="V30" s="4">
+        <v>18</v>
+      </c>
+      <c r="W30" s="4">
         <v>28</v>
       </c>
     </row>
-    <row r="30">
-      <c r="H30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="4">
+    <row r="31">
+      <c r="G31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="4">
         <v>1</v>
       </c>
-      <c r="J30" s="4">
-        <v>3</v>
-      </c>
-      <c r="K30" s="4">
-        <v>3</v>
-      </c>
-      <c r="T30" s="2">
-        <v>2</v>
-      </c>
-      <c r="U30" s="2">
-        <v>7</v>
-      </c>
-      <c r="V30" s="2">
-        <v>18</v>
-      </c>
-      <c r="W30" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="H31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="4">
-        <v>4</v>
-      </c>
       <c r="J31" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K31" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T31" s="2">
         <v>2</v>
@@ -1776,21 +1837,24 @@
         <v>18</v>
       </c>
       <c r="W31" s="4">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32">
+      <c r="G32" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H32" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I32" s="4">
+        <v>4</v>
+      </c>
+      <c r="J32" s="4">
+        <v>5</v>
+      </c>
+      <c r="K32" s="4">
         <v>6</v>
-      </c>
-      <c r="J32" s="4">
-        <v>30</v>
-      </c>
-      <c r="K32" s="4">
-        <v>8</v>
       </c>
       <c r="T32" s="2">
         <v>2</v>
@@ -1802,94 +1866,76 @@
         <v>18</v>
       </c>
       <c r="W32" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="4">
+        <v>6</v>
+      </c>
+      <c r="J33" s="4">
+        <v>30</v>
+      </c>
+      <c r="K33" s="4">
+        <v>8</v>
+      </c>
+      <c r="T33" s="2">
+        <v>2</v>
+      </c>
+      <c r="U33" s="2">
+        <v>7</v>
+      </c>
+      <c r="V33" s="2">
+        <v>18</v>
+      </c>
+      <c r="W33" s="4">
         <v>31</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="4" t="s">
+    <row r="34" s="10" customFormat="1">
+      <c r="T34" s="10">
+        <v>2</v>
+      </c>
+      <c r="U34" s="10">
+        <v>7</v>
+      </c>
+      <c r="V34" s="10">
+        <v>18</v>
+      </c>
+      <c r="W34" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="B35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="4">
-        <v>0</v>
-      </c>
-      <c r="J33" s="4">
-        <v>0</v>
-      </c>
-      <c r="K33" s="4">
-        <v>9</v>
-      </c>
-      <c r="T33" s="4">
-        <v>3</v>
-      </c>
-      <c r="U33" s="4">
-        <v>8</v>
-      </c>
-      <c r="V33" s="4">
-        <v>19</v>
-      </c>
-      <c r="W33" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="E34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="4">
-        <v>0</v>
-      </c>
-      <c r="J34" s="4">
-        <v>0</v>
-      </c>
-      <c r="K34" s="4">
-        <v>1</v>
-      </c>
-      <c r="T34" s="2">
-        <v>3</v>
-      </c>
-      <c r="U34" s="2">
-        <v>8</v>
-      </c>
-      <c r="V34" s="4">
-        <v>20</v>
-      </c>
-      <c r="W34" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35">
+      <c r="D35" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="E35" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G35" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H35" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I35" s="4">
         <v>0</v>
@@ -1900,40 +1946,31 @@
       <c r="K35" s="4">
         <v>9</v>
       </c>
-      <c r="T35" s="2">
-        <v>3</v>
-      </c>
-      <c r="U35" s="2">
+      <c r="T35" s="4">
+        <v>3</v>
+      </c>
+      <c r="U35" s="4">
         <v>8</v>
       </c>
       <c r="V35" s="4">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="W35" s="4">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="E36" s="4" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I36" s="4">
         <v>0</v>
@@ -1942,85 +1979,106 @@
         <v>0</v>
       </c>
       <c r="K36" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T36" s="2">
         <v>3</v>
       </c>
-      <c r="U36" s="4">
-        <v>9</v>
+      <c r="U36" s="2">
+        <v>8</v>
       </c>
       <c r="V36" s="4">
+        <v>20</v>
+      </c>
+      <c r="W36" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0</v>
+      </c>
+      <c r="J37" s="4">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4">
+        <v>9</v>
+      </c>
+      <c r="T37" s="2">
+        <v>3</v>
+      </c>
+      <c r="U37" s="2">
+        <v>8</v>
+      </c>
+      <c r="V37" s="4">
+        <v>21</v>
+      </c>
+      <c r="W37" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0</v>
+      </c>
+      <c r="J38" s="4">
+        <v>0</v>
+      </c>
+      <c r="K38" s="4">
+        <v>2</v>
+      </c>
+      <c r="T38" s="2">
+        <v>3</v>
+      </c>
+      <c r="U38" s="4">
+        <v>9</v>
+      </c>
+      <c r="V38" s="4">
         <v>22</v>
       </c>
-      <c r="W36" s="4">
+      <c r="W38" s="4">
         <v>35</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="G37" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="4">
-        <v>0</v>
-      </c>
-      <c r="J37" s="4">
-        <v>0</v>
-      </c>
-      <c r="K37" s="4">
-        <v>2</v>
-      </c>
-      <c r="T37" s="2">
-        <v>3</v>
-      </c>
-      <c r="U37" s="2">
-        <v>9</v>
-      </c>
-      <c r="V37" s="2">
-        <v>22</v>
-      </c>
-      <c r="W37" s="4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="G38" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="4">
-        <v>0</v>
-      </c>
-      <c r="J38" s="4">
-        <v>0</v>
-      </c>
-      <c r="K38" s="4">
-        <v>7</v>
-      </c>
-      <c r="T38" s="2">
-        <v>3</v>
-      </c>
-      <c r="U38" s="2">
-        <v>9</v>
-      </c>
-      <c r="V38" s="2">
-        <v>22</v>
-      </c>
-      <c r="W38" s="4">
-        <v>37</v>
       </c>
     </row>
     <row r="39">
       <c r="G39" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I39" s="4">
         <v>0</v>
@@ -2029,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="T39" s="2">
         <v>3</v>
@@ -2041,15 +2099,15 @@
         <v>22</v>
       </c>
       <c r="W39" s="4">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40">
       <c r="G40" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I40" s="4">
         <v>0</v>
@@ -2058,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T40" s="2">
         <v>3</v>
@@ -2070,15 +2128,15 @@
         <v>22</v>
       </c>
       <c r="W40" s="4">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41">
       <c r="G41" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I41" s="4">
         <v>0</v>
@@ -2087,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T41" s="2">
         <v>3</v>
@@ -2099,15 +2157,15 @@
         <v>22</v>
       </c>
       <c r="W41" s="4">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42">
       <c r="G42" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I42" s="4">
         <v>0</v>
@@ -2116,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T42" s="2">
         <v>3</v>
@@ -2128,15 +2186,15 @@
         <v>22</v>
       </c>
       <c r="W42" s="4">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43">
       <c r="G43" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I43" s="4">
         <v>0</v>
@@ -2145,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T43" s="2">
         <v>3</v>
@@ -2157,140 +2215,143 @@
         <v>22</v>
       </c>
       <c r="W43" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="G44" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="4">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4">
+        <v>1</v>
+      </c>
+      <c r="T44" s="2">
+        <v>3</v>
+      </c>
+      <c r="U44" s="2">
+        <v>9</v>
+      </c>
+      <c r="V44" s="2">
+        <v>22</v>
+      </c>
+      <c r="W44" s="4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="G45" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4">
+        <v>0</v>
+      </c>
+      <c r="K45" s="4">
+        <v>1</v>
+      </c>
+      <c r="T45" s="2">
+        <v>3</v>
+      </c>
+      <c r="U45" s="2">
+        <v>9</v>
+      </c>
+      <c r="V45" s="2">
+        <v>22</v>
+      </c>
+      <c r="W45" s="4">
         <v>42</v>
       </c>
     </row>
-    <row r="44">
-      <c r="E44" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F44" s="4" t="s">
+    <row r="46">
+      <c r="E46" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H44" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" s="4">
-        <v>0</v>
-      </c>
-      <c r="J44" s="4">
-        <v>0</v>
-      </c>
-      <c r="K44" s="4">
-        <v>9</v>
-      </c>
-      <c r="T44" s="2">
-        <v>3</v>
-      </c>
-      <c r="U44" s="2">
-        <v>9</v>
-      </c>
-      <c r="V44" s="4">
+      <c r="G46" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="4">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4">
+        <v>9</v>
+      </c>
+      <c r="T46" s="2">
+        <v>3</v>
+      </c>
+      <c r="U46" s="2">
+        <v>9</v>
+      </c>
+      <c r="V46" s="4">
         <v>23</v>
       </c>
-      <c r="W44" s="4">
+      <c r="W46" s="4">
         <v>43</v>
       </c>
     </row>
-    <row r="45">
-      <c r="E45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F45" s="4" t="s">
+    <row r="47">
+      <c r="E47" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G47" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0</v>
+      </c>
+      <c r="J47" s="4">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4">
+        <v>2</v>
+      </c>
+      <c r="T47" s="2">
+        <v>3</v>
+      </c>
+      <c r="U47" s="2">
+        <v>9</v>
+      </c>
+      <c r="V47" s="4">
         <v>24</v>
       </c>
-      <c r="H45" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I45" s="4">
-        <v>0</v>
-      </c>
-      <c r="J45" s="4">
-        <v>0</v>
-      </c>
-      <c r="K45" s="4">
-        <v>2</v>
-      </c>
-      <c r="T45" s="2">
-        <v>3</v>
-      </c>
-      <c r="U45" s="2">
-        <v>9</v>
-      </c>
-      <c r="V45" s="4">
-        <v>24</v>
-      </c>
-      <c r="W45" s="4">
+      <c r="W47" s="4">
         <v>44</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="G46" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I46" s="4">
-        <v>0</v>
-      </c>
-      <c r="J46" s="4">
-        <v>0</v>
-      </c>
-      <c r="K46" s="4">
-        <v>2</v>
-      </c>
-      <c r="T46" s="2">
-        <v>3</v>
-      </c>
-      <c r="U46" s="2">
-        <v>9</v>
-      </c>
-      <c r="V46" s="2">
-        <v>24</v>
-      </c>
-      <c r="W46" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="G47" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="4">
-        <v>0</v>
-      </c>
-      <c r="J47" s="4">
-        <v>0</v>
-      </c>
-      <c r="K47" s="4">
-        <v>7</v>
-      </c>
-      <c r="T47" s="2">
-        <v>3</v>
-      </c>
-      <c r="U47" s="2">
-        <v>9</v>
-      </c>
-      <c r="V47" s="2">
-        <v>24</v>
-      </c>
-      <c r="W47" s="4">
-        <v>46</v>
       </c>
     </row>
     <row r="48">
       <c r="G48" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I48" s="4">
         <v>0</v>
@@ -2299,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="K48" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="T48" s="2">
         <v>3</v>
@@ -2311,15 +2372,15 @@
         <v>24</v>
       </c>
       <c r="W48" s="4">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49">
       <c r="G49" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I49" s="4">
         <v>0</v>
@@ -2328,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="K49" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T49" s="2">
         <v>3</v>
@@ -2340,15 +2401,15 @@
         <v>24</v>
       </c>
       <c r="W49" s="4">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50">
       <c r="G50" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I50" s="4">
         <v>0</v>
@@ -2357,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="K50" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T50" s="2">
         <v>3</v>
@@ -2369,15 +2430,15 @@
         <v>24</v>
       </c>
       <c r="W50" s="4">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51">
       <c r="G51" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I51" s="4">
         <v>0</v>
@@ -2386,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T51" s="2">
         <v>3</v>
@@ -2398,15 +2459,15 @@
         <v>24</v>
       </c>
       <c r="W51" s="4">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52">
       <c r="G52" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I52" s="4">
         <v>0</v>
@@ -2415,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T52" s="2">
         <v>3</v>
@@ -2427,108 +2488,108 @@
         <v>24</v>
       </c>
       <c r="W52" s="4">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53">
-      <c r="E53" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="G53" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+      <c r="J53" s="4">
+        <v>0</v>
+      </c>
+      <c r="K53" s="4">
+        <v>1</v>
+      </c>
+      <c r="T53" s="2">
+        <v>3</v>
+      </c>
+      <c r="U53" s="2">
+        <v>9</v>
+      </c>
+      <c r="V53" s="2">
         <v>24</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I53" s="4">
-        <v>0</v>
-      </c>
-      <c r="J53" s="4">
-        <v>0</v>
-      </c>
-      <c r="K53" s="4">
-        <v>3</v>
-      </c>
-      <c r="T53" s="2">
-        <v>3</v>
-      </c>
-      <c r="U53" s="2">
-        <v>9</v>
-      </c>
-      <c r="V53" s="4">
-        <v>25</v>
-      </c>
       <c r="W53" s="4">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54">
       <c r="G54" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
+      <c r="J54" s="4">
+        <v>0</v>
+      </c>
+      <c r="K54" s="4">
+        <v>1</v>
+      </c>
+      <c r="T54" s="2">
+        <v>3</v>
+      </c>
+      <c r="U54" s="2">
+        <v>9</v>
+      </c>
+      <c r="V54" s="2">
+        <v>24</v>
+      </c>
+      <c r="W54" s="4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="E55" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H54" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I54" s="4">
-        <v>0</v>
-      </c>
-      <c r="J54" s="4">
-        <v>0</v>
-      </c>
-      <c r="K54" s="4">
-        <v>3</v>
-      </c>
-      <c r="T54" s="2">
-        <v>3</v>
-      </c>
-      <c r="U54" s="2">
-        <v>9</v>
-      </c>
-      <c r="V54" s="2">
+      <c r="H55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0</v>
+      </c>
+      <c r="J55" s="4">
+        <v>0</v>
+      </c>
+      <c r="K55" s="4">
+        <v>3</v>
+      </c>
+      <c r="T55" s="2">
+        <v>3</v>
+      </c>
+      <c r="U55" s="2">
+        <v>9</v>
+      </c>
+      <c r="V55" s="4">
         <v>25</v>
       </c>
-      <c r="W54" s="4">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="G55" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I55" s="4">
-        <v>0</v>
-      </c>
-      <c r="J55" s="4">
-        <v>0</v>
-      </c>
-      <c r="K55" s="4">
-        <v>8</v>
-      </c>
-      <c r="T55" s="2">
-        <v>3</v>
-      </c>
-      <c r="U55" s="2">
-        <v>9</v>
-      </c>
-      <c r="V55" s="2">
-        <v>25</v>
-      </c>
       <c r="W55" s="4">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56">
       <c r="G56" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I56" s="4">
         <v>0</v>
@@ -2537,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="T56" s="2">
         <v>3</v>
@@ -2549,15 +2610,15 @@
         <v>25</v>
       </c>
       <c r="W56" s="4">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57">
       <c r="G57" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I57" s="4">
         <v>0</v>
@@ -2566,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="K57" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T57" s="2">
         <v>3</v>
@@ -2578,15 +2639,15 @@
         <v>25</v>
       </c>
       <c r="W57" s="4">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58">
       <c r="G58" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I58" s="4">
         <v>0</v>
@@ -2595,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="K58" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T58" s="2">
         <v>3</v>
@@ -2607,15 +2668,15 @@
         <v>25</v>
       </c>
       <c r="W58" s="4">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59">
       <c r="G59" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I59" s="4">
         <v>0</v>
@@ -2624,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="K59" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="T59" s="2">
         <v>3</v>
@@ -2636,15 +2697,15 @@
         <v>25</v>
       </c>
       <c r="W59" s="4">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60">
       <c r="G60" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I60" s="4">
         <v>0</v>
@@ -2653,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="K60" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="T60" s="2">
         <v>3</v>
@@ -2665,126 +2726,105 @@
         <v>25</v>
       </c>
       <c r="W60" s="4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="G61" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" s="4">
+        <v>0</v>
+      </c>
+      <c r="J61" s="4">
+        <v>0</v>
+      </c>
+      <c r="K61" s="4">
+        <v>2</v>
+      </c>
+      <c r="T61" s="2">
+        <v>3</v>
+      </c>
+      <c r="U61" s="2">
+        <v>9</v>
+      </c>
+      <c r="V61" s="2">
+        <v>25</v>
+      </c>
+      <c r="W61" s="4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="G62" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0</v>
+      </c>
+      <c r="J62" s="4">
+        <v>0</v>
+      </c>
+      <c r="K62" s="4">
+        <v>2</v>
+      </c>
+      <c r="T62" s="2">
+        <v>3</v>
+      </c>
+      <c r="U62" s="2">
+        <v>9</v>
+      </c>
+      <c r="V62" s="2">
+        <v>25</v>
+      </c>
+      <c r="W62" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="4" t="s">
+    <row r="63" s="10" customFormat="1">
+      <c r="T63" s="10">
+        <v>3</v>
+      </c>
+      <c r="U63" s="10">
+        <v>9</v>
+      </c>
+      <c r="V63" s="10">
+        <v>25</v>
+      </c>
+      <c r="W63" s="10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="4" t="s">
+      <c r="B64" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I61" s="4">
-        <v>0</v>
-      </c>
-      <c r="J61" s="4">
-        <v>0</v>
-      </c>
-      <c r="K61" s="4">
-        <v>9</v>
-      </c>
-      <c r="T61" s="4">
-        <v>4</v>
-      </c>
-      <c r="U61" s="4">
-        <v>10</v>
-      </c>
-      <c r="V61" s="4">
-        <v>26</v>
-      </c>
-      <c r="W61" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="E62" s="4" t="s">
+      <c r="E64" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I62" s="4">
-        <v>0</v>
-      </c>
-      <c r="J62" s="4">
-        <v>0</v>
-      </c>
-      <c r="K62" s="4">
-        <v>9</v>
-      </c>
-      <c r="T62" s="2">
-        <v>4</v>
-      </c>
-      <c r="U62" s="2">
-        <v>10</v>
-      </c>
-      <c r="V62" s="4">
-        <v>27</v>
-      </c>
-      <c r="W62" s="4">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="E63" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I63" s="4">
-        <v>0</v>
-      </c>
-      <c r="J63" s="4">
-        <v>0</v>
-      </c>
-      <c r="K63" s="4">
-        <v>1</v>
-      </c>
-      <c r="T63" s="2">
-        <v>4</v>
-      </c>
-      <c r="U63" s="2">
-        <v>10</v>
-      </c>
-      <c r="V63" s="4">
-        <v>28</v>
-      </c>
-      <c r="W63" s="4">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="E64" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G64" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H64" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I64" s="4">
         <v>0</v>
@@ -2795,37 +2835,31 @@
       <c r="K64" s="4">
         <v>9</v>
       </c>
-      <c r="T64" s="2">
+      <c r="T64" s="4">
         <v>4</v>
       </c>
-      <c r="U64" s="2">
+      <c r="U64" s="4">
         <v>10</v>
       </c>
       <c r="V64" s="4">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="W64" s="4">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65">
-      <c r="B65" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="E65" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G65" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H65" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I65" s="4">
         <v>0</v>
@@ -2834,30 +2868,33 @@
         <v>0</v>
       </c>
       <c r="K65" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="T65" s="2">
         <v>4</v>
       </c>
-      <c r="U65" s="4">
-        <v>11</v>
+      <c r="U65" s="2">
+        <v>10</v>
       </c>
       <c r="V65" s="4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="W65" s="4">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66">
       <c r="E66" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G66" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H66" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I66" s="4">
         <v>0</v>
@@ -2872,24 +2909,27 @@
         <v>4</v>
       </c>
       <c r="U66" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V66" s="4">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="W66" s="4">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67">
       <c r="E67" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G67" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H67" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I67" s="4">
         <v>0</v>
@@ -2898,391 +2938,415 @@
         <v>0</v>
       </c>
       <c r="K67" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="T67" s="2">
         <v>4</v>
       </c>
       <c r="U67" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V67" s="4">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="W67" s="4">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>35</v>
+        <v>14</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I68" s="4">
         <v>0</v>
       </c>
       <c r="J68" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K68" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="T68" s="2">
         <v>4</v>
       </c>
       <c r="U68" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V68" s="4">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="W68" s="4">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69">
+      <c r="E69" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H69" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I69" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J69" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K69" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T69" s="2">
         <v>4</v>
       </c>
       <c r="U69" s="2">
-        <v>12</v>
-      </c>
-      <c r="V69" s="2">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="V69" s="4">
+        <v>31</v>
       </c>
       <c r="W69" s="4">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70">
-      <c r="B70" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>35</v>
+      <c r="E70" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I70" s="4">
         <v>0</v>
       </c>
       <c r="J70" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K70" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="T70" s="2">
         <v>4</v>
       </c>
-      <c r="U70" s="4">
-        <v>13</v>
+      <c r="U70" s="2">
+        <v>11</v>
       </c>
       <c r="V70" s="4">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W70" s="4">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71">
+      <c r="B71" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H71" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I71" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J71" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K71" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T71" s="2">
         <v>4</v>
       </c>
-      <c r="U71" s="2">
-        <v>13</v>
-      </c>
-      <c r="V71" s="2">
-        <v>34</v>
+      <c r="U71" s="4">
+        <v>12</v>
+      </c>
+      <c r="V71" s="4">
+        <v>33</v>
       </c>
       <c r="W71" s="4">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72">
-      <c r="B72" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>36</v>
+      <c r="G72" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I72" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J72" s="4">
+        <v>10</v>
+      </c>
+      <c r="K72" s="4">
         <v>5</v>
-      </c>
-      <c r="K72" s="4">
-        <v>1</v>
       </c>
       <c r="T72" s="2">
         <v>4</v>
       </c>
-      <c r="U72" s="4">
-        <v>14</v>
-      </c>
-      <c r="V72" s="4">
+      <c r="U72" s="2">
+        <v>12</v>
+      </c>
+      <c r="V72" s="2">
+        <v>33</v>
+      </c>
+      <c r="W72" s="4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="W72" s="4">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73">
+      <c r="D73" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H73" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I73" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J73" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K73" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="T73" s="2">
         <v>4</v>
       </c>
-      <c r="U73" s="2">
+      <c r="U73" s="4">
+        <v>13</v>
+      </c>
+      <c r="V73" s="4">
+        <v>34</v>
+      </c>
+      <c r="W73" s="4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="G74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I74" s="4">
+        <v>6</v>
+      </c>
+      <c r="J74" s="4">
+        <v>10</v>
+      </c>
+      <c r="K74" s="4">
+        <v>8</v>
+      </c>
+      <c r="T74" s="2">
+        <v>4</v>
+      </c>
+      <c r="U74" s="2">
+        <v>13</v>
+      </c>
+      <c r="V74" s="2">
+        <v>34</v>
+      </c>
+      <c r="W74" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" s="4">
+        <v>0</v>
+      </c>
+      <c r="J75" s="4">
+        <v>5</v>
+      </c>
+      <c r="K75" s="4">
+        <v>1</v>
+      </c>
+      <c r="T75" s="2">
+        <v>4</v>
+      </c>
+      <c r="U75" s="4">
         <v>14</v>
       </c>
-      <c r="V73" s="2">
+      <c r="V75" s="4">
         <v>35</v>
       </c>
-      <c r="W73" s="4">
+      <c r="W75" s="4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="G76" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I76" s="4">
+        <v>6</v>
+      </c>
+      <c r="J76" s="4">
+        <v>10</v>
+      </c>
+      <c r="K76" s="4">
+        <v>7</v>
+      </c>
+      <c r="T76" s="2">
+        <v>4</v>
+      </c>
+      <c r="U76" s="2">
+        <v>14</v>
+      </c>
+      <c r="V76" s="2">
+        <v>35</v>
+      </c>
+      <c r="W76" s="4">
         <v>72</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B74" s="4" t="s">
+    <row r="77" s="10" customFormat="1">
+      <c r="T77" s="10">
+        <v>4</v>
+      </c>
+      <c r="U77" s="10">
+        <v>14</v>
+      </c>
+      <c r="V77" s="10">
+        <v>35</v>
+      </c>
+      <c r="W77" s="10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D74" s="4" t="s">
+      <c r="B78" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="D78" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H74" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I74" s="4">
-        <v>0</v>
-      </c>
-      <c r="J74" s="4">
+      <c r="F78" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I78" s="4">
+        <v>0</v>
+      </c>
+      <c r="J78" s="4">
         <v>200</v>
-      </c>
-      <c r="K74" s="4">
-        <v>1</v>
-      </c>
-      <c r="T74" s="4">
-        <v>5</v>
-      </c>
-      <c r="U74" s="4">
-        <v>15</v>
-      </c>
-      <c r="V74" s="4">
-        <v>36</v>
-      </c>
-      <c r="W74" s="4">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="H75" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I75" s="4">
-        <v>201</v>
-      </c>
-      <c r="J75" s="4">
-        <v>1000</v>
-      </c>
-      <c r="K75" s="4">
-        <v>9</v>
-      </c>
-      <c r="T75" s="2">
-        <v>5</v>
-      </c>
-      <c r="U75" s="2">
-        <v>15</v>
-      </c>
-      <c r="V75" s="2">
-        <v>36</v>
-      </c>
-      <c r="W75" s="4">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I76" s="4">
-        <v>0</v>
-      </c>
-      <c r="J76" s="4">
-        <v>24</v>
-      </c>
-      <c r="K76" s="4">
-        <v>1</v>
-      </c>
-      <c r="T76" s="2">
-        <v>5</v>
-      </c>
-      <c r="U76" s="4">
-        <v>16</v>
-      </c>
-      <c r="V76" s="4">
-        <v>37</v>
-      </c>
-      <c r="W76" s="4">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="H77" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I77" s="4">
-        <v>25</v>
-      </c>
-      <c r="J77" s="4">
-        <v>100</v>
-      </c>
-      <c r="K77" s="4">
-        <v>9</v>
-      </c>
-      <c r="T77" s="2">
-        <v>5</v>
-      </c>
-      <c r="U77" s="2">
-        <v>16</v>
-      </c>
-      <c r="V77" s="2">
-        <v>37</v>
-      </c>
-      <c r="W77" s="4">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H78" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I78" s="4">
-        <v>0</v>
-      </c>
-      <c r="J78" s="4">
-        <v>100</v>
       </c>
       <c r="K78" s="4">
         <v>1</v>
       </c>
-      <c r="T78" s="2">
+      <c r="T78" s="4">
         <v>5</v>
       </c>
       <c r="U78" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="V78" s="4">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="W78" s="4">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79">
+      <c r="G79" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H79" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I79" s="4">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="J79" s="4">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="K79" s="4">
         <v>9</v>
@@ -3291,36 +3355,39 @@
         <v>5</v>
       </c>
       <c r="U79" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="V79" s="2">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="W79" s="4">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I80" s="4">
         <v>0</v>
       </c>
       <c r="J80" s="4">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="K80" s="4">
         <v>1</v>
@@ -3329,24 +3396,27 @@
         <v>5</v>
       </c>
       <c r="U80" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="V80" s="4">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="W80" s="4">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81">
+      <c r="G81" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H81" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I81" s="4">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="J81" s="4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="K81" s="4">
         <v>9</v>
@@ -3355,100 +3425,109 @@
         <v>5</v>
       </c>
       <c r="U81" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="V81" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="W81" s="4">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I82" s="4">
         <v>0</v>
       </c>
       <c r="J82" s="4">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K82" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="T82" s="2">
         <v>5</v>
       </c>
       <c r="U82" s="4">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="V82" s="4">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="W82" s="4">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83">
+      <c r="G83" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H83" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I83" s="4">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="J83" s="4">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="K83" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T83" s="2">
         <v>5</v>
       </c>
       <c r="U83" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="V83" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="W83" s="4">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I84" s="4">
+        <v>0</v>
+      </c>
+      <c r="J84" s="4">
         <v>79</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H84" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I84" s="4">
-        <v>0</v>
-      </c>
-      <c r="J84" s="4">
-        <v>100</v>
       </c>
       <c r="K84" s="4">
         <v>1</v>
@@ -3457,24 +3536,27 @@
         <v>5</v>
       </c>
       <c r="U84" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="V84" s="4">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="W84" s="4">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85">
+      <c r="G85" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H85" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I85" s="4">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="J85" s="4">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K85" s="4">
         <v>9</v>
@@ -3483,36 +3565,39 @@
         <v>5</v>
       </c>
       <c r="U85" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="V85" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="W85" s="4">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I86" s="4">
+        <v>0</v>
+      </c>
+      <c r="J86" s="4">
         <v>80</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H86" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I86" s="4">
-        <v>0</v>
-      </c>
-      <c r="J86" s="4">
-        <v>40</v>
       </c>
       <c r="K86" s="4">
         <v>9</v>
@@ -3521,50 +3606,68 @@
         <v>5</v>
       </c>
       <c r="U86" s="4">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="V86" s="4">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="W86" s="4">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87">
+      <c r="G87" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H87" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I87" s="4">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="J87" s="4">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="K87" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="T87" s="2">
         <v>5</v>
       </c>
       <c r="U87" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="V87" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="W87" s="4">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88">
+      <c r="B88" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H88" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I88" s="4">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J88" s="4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="K88" s="4">
         <v>1</v>
@@ -3572,40 +3675,43 @@
       <c r="T88" s="2">
         <v>5</v>
       </c>
-      <c r="U88" s="2">
-        <v>21</v>
-      </c>
-      <c r="V88" s="2">
-        <v>42</v>
+      <c r="U88" s="4">
+        <v>20</v>
+      </c>
+      <c r="V88" s="4">
+        <v>41</v>
       </c>
       <c r="W88" s="4">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89">
+      <c r="G89" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H89" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I89" s="4">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="J89" s="4">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="K89" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T89" s="2">
         <v>5</v>
       </c>
       <c r="U89" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V89" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W89" s="4">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90">
@@ -3613,48 +3719,54 @@
         <v>81</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I90" s="4">
         <v>0</v>
       </c>
       <c r="J90" s="4">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="K90" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T90" s="2">
         <v>5</v>
       </c>
       <c r="U90" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V90" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W90" s="4">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91">
+      <c r="G91" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H91" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I91" s="4">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="J91" s="4">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="K91" s="4">
         <v>9</v>
@@ -3663,36 +3775,27 @@
         <v>5</v>
       </c>
       <c r="U91" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V91" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W91" s="4">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92">
-      <c r="B92" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>36</v>
+      <c r="G92" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I92" s="4">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J92" s="4">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="K92" s="4">
         <v>1</v>
@@ -3700,39 +3803,182 @@
       <c r="T92" s="2">
         <v>5</v>
       </c>
-      <c r="U92" s="4">
-        <v>23</v>
-      </c>
-      <c r="V92" s="4">
-        <v>44</v>
+      <c r="U92" s="2">
+        <v>21</v>
+      </c>
+      <c r="V92" s="2">
+        <v>42</v>
       </c>
       <c r="W92" s="4">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93">
+      <c r="G93" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H93" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I93" s="4">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="J93" s="4">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="K93" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="T93" s="2">
         <v>5</v>
       </c>
       <c r="U93" s="2">
+        <v>21</v>
+      </c>
+      <c r="V93" s="2">
+        <v>42</v>
+      </c>
+      <c r="W93" s="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I94" s="4">
+        <v>0</v>
+      </c>
+      <c r="J94" s="4">
+        <v>150</v>
+      </c>
+      <c r="K94" s="4">
+        <v>1</v>
+      </c>
+      <c r="T94" s="2">
+        <v>5</v>
+      </c>
+      <c r="U94" s="4">
+        <v>22</v>
+      </c>
+      <c r="V94" s="4">
+        <v>43</v>
+      </c>
+      <c r="W94" s="4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="G95" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I95" s="4">
+        <v>151</v>
+      </c>
+      <c r="J95" s="4">
+        <v>400</v>
+      </c>
+      <c r="K95" s="4">
+        <v>9</v>
+      </c>
+      <c r="T95" s="2">
+        <v>5</v>
+      </c>
+      <c r="U95" s="2">
+        <v>22</v>
+      </c>
+      <c r="V95" s="2">
+        <v>43</v>
+      </c>
+      <c r="W95" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I96" s="4">
+        <v>0</v>
+      </c>
+      <c r="J96" s="4">
+        <v>150</v>
+      </c>
+      <c r="K96" s="4">
+        <v>1</v>
+      </c>
+      <c r="T96" s="2">
+        <v>5</v>
+      </c>
+      <c r="U96" s="4">
         <v>23</v>
       </c>
-      <c r="V93" s="2">
+      <c r="V96" s="4">
         <v>44</v>
       </c>
-      <c r="W93" s="4">
+      <c r="W96" s="4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="G97" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I97" s="4">
+        <v>151</v>
+      </c>
+      <c r="J97" s="4">
+        <v>300</v>
+      </c>
+      <c r="K97" s="4">
+        <v>9</v>
+      </c>
+      <c r="T97" s="2">
+        <v>5</v>
+      </c>
+      <c r="U97" s="2">
+        <v>23</v>
+      </c>
+      <c r="V97" s="2">
+        <v>44</v>
+      </c>
+      <c r="W97" s="4">
         <v>92</v>
       </c>
     </row>
@@ -3763,7 +4009,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Valori Ammissibili'!$C$2:$C$9</xm:f>
+            <xm:f>'Valori Ammissibili'!$C$2:$C$10</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
@@ -3784,7 +4030,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3800,16 +4046,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
@@ -3820,27 +4066,27 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
@@ -3848,71 +4094,74 @@
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="D10" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
       <c r="D11" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
       <c r="D12" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>